<commit_message>
Sums and its Patterns
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/namankothari/Documents/Naman Kothari/Leetcode_Solutions/Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B0D532E-752A-114A-A574-7071154C2ED9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60A3F46E-EA21-EB43-8B05-6CFA49A11551}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3480" yWindow="2560" windowWidth="27640" windowHeight="16940" xr2:uid="{C34AE6C3-BFC3-4D45-AF40-CB304CD30E76}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="65">
   <si>
     <t>Binary Search Tree</t>
   </si>
@@ -44,9 +44,6 @@
     <t>Things I learned</t>
   </si>
   <si>
-    <t>Topics</t>
-  </si>
-  <si>
     <t>1- The right and left child of each node are STRICTLY less than or greater than THERE IS NO EQUAL TO.</t>
   </si>
   <si>
@@ -69,6 +66,209 @@
   </si>
   <si>
     <t>ABSOLUTE KEY REMINDER --&gt; PREORDER, INORDER, POSTORDER are ALL just values in a LIST and not NODES!</t>
+  </si>
+  <si>
+    <t>Topics(structure)</t>
+  </si>
+  <si>
+    <t>sum specific</t>
+  </si>
+  <si>
+    <t>maxsumpath</t>
+  </si>
+  <si>
+    <t>A path can also ONLY CONSIST OF THE NODE ITSELF if THAT NODE BY ITSELF IS GREATER THAN ANY OTHER NODES IN ANY PATH (BASICALLY A NODE BY ITSELF IS ALSO A PATH)</t>
+  </si>
+  <si>
+    <t>When numbers are in negative and writing a recursive function, be aware of the base condition if it inlcudes numbers like 0 or anything cause negative numbers will be over-ruled by 0's base condition and the answer will come wrong.</t>
+  </si>
+  <si>
+    <t>IF you are considering left_combined nodes values and right_combined nodes values, do not forget that the root node byitself can also be greater than both of these and so root_combined should also be assessed</t>
+  </si>
+  <si>
+    <t>Binary Tree</t>
+  </si>
+  <si>
+    <t>A binary tree can be reconstructued only using the preorder or inorder or postorder list, just make sure that the nulls are present in the list, if they are not then you will need atleast two of the above in order to be able to reconstruct the tree.</t>
+  </si>
+  <si>
+    <t>I know for sure that preorder and inorder can provide you enough info together (IF BOTH DON’T HAVE NULLS REPRESENTED WITHIN THEM) to make you able to create a binary tree.</t>
+  </si>
+  <si>
+    <t>Serialization</t>
+  </si>
+  <si>
+    <t>Serialization is the conversion of ANY DATA STRUCTURE (usually complex) into a single string or into its binary representation and then passing it over the network/medium so as to be able to transfer same info with less utiization of the net.</t>
+  </si>
+  <si>
+    <t>Famous Reasons for using this DS:</t>
+  </si>
+  <si>
+    <t>Heap</t>
+  </si>
+  <si>
+    <t>Dijkstra</t>
+  </si>
+  <si>
+    <t>Median of a Stream</t>
+  </si>
+  <si>
+    <t>Traversals(Pre-Order, Post-Order, In-Order, Level Order)  - Lowest Common Ancestor</t>
+  </si>
+  <si>
+    <t>Left View of a Binary Tree,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Maximum Path Sum</t>
+  </si>
+  <si>
+    <t>heap sort</t>
+  </si>
+  <si>
+    <t>Hashmap</t>
+  </si>
+  <si>
+    <t>Whenever a quick lookup is needed</t>
+  </si>
+  <si>
+    <t>Stack/Queue</t>
+  </si>
+  <si>
+    <t>Largest Rectangle in a Histogram</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Graphs </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Graph Search(BFS, DFS, Dijkstra), </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Topological Sort, </t>
+  </si>
+  <si>
+    <t>Loop in a Graph - Bus Routes</t>
+  </si>
+  <si>
+    <t>Use stack when you are going throigh a bunch of values and you see that you will always require the last seen element the first then use Stack.</t>
+  </si>
+  <si>
+    <t>THIS IS THE MOST DIFF DS to identify, so work on identifying this the most for practise</t>
+  </si>
+  <si>
+    <t>BFS and Dijkstra are used the find the shortest path between two nodes in a graph</t>
+  </si>
+  <si>
+    <t>Remember that heap is ALWAYS a complete binary tree</t>
+  </si>
+  <si>
+    <t>1- you can find the amount in just 1 position in the array by simply subtracting the element present at position I - the element at position i-1</t>
+  </si>
+  <si>
+    <t>2- to find the sum of elements from posititon x to position y in an array then you onky need to subtract value at position y - value at position x-1</t>
+  </si>
+  <si>
+    <t>eg:-</t>
+  </si>
+  <si>
+    <t>Observations:-</t>
+  </si>
+  <si>
+    <t>Prefix Sumarray</t>
+  </si>
+  <si>
+    <t>use a prefix sum array of type long cause int can overflow if the numbers we are adding go beyond 10^5</t>
+  </si>
+  <si>
+    <t>1- (KADANE's ALgo)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maximum Subarray, </t>
+  </si>
+  <si>
+    <t>for example if I give you list of lists which contains [I,j] and I is indicating the index at which you want to do the addition till the end of the array and j is the number you want to add</t>
+  </si>
+  <si>
+    <t>addition of numbers from index I to n-1 in an array. --&gt; Question here --&gt;</t>
+  </si>
+  <si>
+    <t>For a particular number, you want to find if the sum of all the numbers on its left and the sum of all the numbers on its right and if they are equal, then that number is called equilibrium number.</t>
+  </si>
+  <si>
+    <t>SUBARRAY</t>
+  </si>
+  <si>
+    <t>Google/meta question regarding it.</t>
+  </si>
+  <si>
+    <t>contribution technique (think rather how many times it appeared in each subarray rather than trying to solve it with prefix sum or anything.)</t>
+  </si>
+  <si>
+    <t>Techniques which are used across multiple DS:-</t>
+  </si>
+  <si>
+    <t>Contribution Technique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eg question: </t>
+  </si>
+  <si>
+    <t>How to recognize the technique:-</t>
+  </si>
+  <si>
+    <t>Types of Questions for Contribution Technique
+	•	Sum of Differences or Distances:
+	•	Problems asking for the sum of differences or distances between elements.
+	•	Example: Sum of absolute differences between all pairs in an array.
+	•	Counting Pairs with Specific Properties:
+	•	Problems where you need to count pairs of elements (i, j) that satisfy certain conditions.
+	•	Example: Count pairs (i, j) such that their sum is divisible by a given number.
+	•	Aggregate Contributions Across Data Structures:
+	•	Problems where each element’s contribution needs to be aggregated across a data structure.
+	•	Example: Total influence of nodes in a graph based on connected edges.
+	•	Bit Manipulation Problems:
+	•	Problems involving bitwise operations where each bit position contributes to the result.
+	•	Example: Sum of different bits between all pairs in an array.
+	•	Geometric Problems:
+	•	Problems involving distances, areas, or other geometric properties.
+	•	Example: Sum of areas of triangles formed by points in a plane.
+	•	Dynamic Programming Problems:
+	•	Problems where contributions from subproblems need to be combined to form the solution.
+	•	Example: Counting paths in a grid where each cell contributes to the paths passing through it.
+	•	Prefix/Suffix Sum Problems:
+	•	Problems where each element’s contribution to prefix or suffix sums needs to be considered.
+	•	Example: Sum of products of all subarrays in an array.
+	•	Graph and Tree Problems:
+	•	Problems where nodes or edges contribute to certain properties like paths or subtrees.
+	•	Example: Sum of distances from each node to all other nodes in a tree.
+	•	Range Queries:
+	•	Problems involving range queries where each element in a range contributes to the result.
+	•	Example: Sum of elements in subarrays or submatrices.
+Key Indicators for Contribution Technique
+	•	Sum or Total:
+	•	The problem asks for a sum or total of some property across elements, pairs, or substructures.
+	•	Repeated Counting:
+	•	Elements, edges, or nodes are considered multiple times across different contexts or subproblems.
+	•	Pairwise Interactions:
+	•	The problem involves interactions or relationships between pairs of elements.
+	•	Bitwise Contributions:
+	•	Each bit position contributes separately to the final result.
+	•	Substructure Contributions:
+	•	Contributions from subarrays, subtrees, or subsets need to be aggregated.</t>
+  </si>
+  <si>
+    <t>if you want to read about it:-</t>
+  </si>
+  <si>
+    <t>https://medium.com/spidernitt/contribution-technique-i-c1730f195b41</t>
+  </si>
+  <si>
+    <t>its called "Find Pivot Index" on leetcode</t>
+  </si>
+  <si>
+    <t>its called "Range Sum Query - Immutable" on leetcode</t>
+  </si>
+  <si>
+    <t>if it was rather from a left to right range instead of n-1 then it is a famous leetcode question called "its called "Range Sum Query - Immutable" on leetcode"</t>
   </si>
 </sst>
 </file>
@@ -124,6 +324,275 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1512548</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>3822700</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>952500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E74BF013-92F7-A980-7888-681292601B0E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10910548" y="10261600"/>
+          <a:ext cx="2310152" cy="1816100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>863600</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>64256</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>3162300</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>609230</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D98F1A25-140C-20B2-5CD4-30EB0FB47FAC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10261600" y="11189456"/>
+          <a:ext cx="2298700" cy="1573674"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2201862</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>5473700</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>487680</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE25565C-A765-CB84-FB81-82E63D848FF4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4932362" y="11595100"/>
+          <a:ext cx="3271838" cy="1744980"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>876299</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>89181</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>5422900</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>156940</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{68899AD9-C029-D081-A9BE-33C543002094}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3606799" y="13678181"/>
+          <a:ext cx="4546601" cy="4741359"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>3339796</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>4889500</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>59942</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C89989A-C18D-F7CC-43AC-40ED8DDAD0DC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12737796" y="12852400"/>
+          <a:ext cx="1549704" cy="923542"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1079500</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>2629204</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>961642</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{917C7E78-BBEE-0B4D-B7E4-2EBEF35C4159}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="21704300" y="800100"/>
+          <a:ext cx="1549704" cy="923542"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -443,65 +912,278 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B3C76B8-389E-4747-9BF7-DE3D6AB721EC}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="44" customWidth="1"/>
-    <col min="2" max="2" width="114" customWidth="1"/>
-    <col min="3" max="3" width="64.33203125" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="19.1640625" customWidth="1"/>
+    <col min="3" max="3" width="87.5" customWidth="1"/>
+    <col min="4" max="4" width="69.1640625" customWidth="1"/>
+    <col min="5" max="5" width="30.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="49" customWidth="1"/>
+    <col min="8" max="8" width="26" customWidth="1"/>
+    <col min="9" max="9" width="54.6640625" customWidth="1"/>
+    <col min="10" max="10" width="58.5" customWidth="1"/>
+    <col min="11" max="11" width="33.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="102" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="E1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J1" t="s">
+        <v>58</v>
+      </c>
+      <c r="K1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="98" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I2" t="s">
+        <v>57</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="K2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+      <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="C5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="B5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
-        <v>9</v>
+    <row r="7" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="C8" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="C9" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E12" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="E14" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="E15" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" t="s">
+        <v>37</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" t="s">
+        <v>39</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="E24" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E25" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>45</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D30" t="s">
+        <v>43</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="81" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>47</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D31" t="s">
+        <v>43</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F31" t="s">
+        <v>49</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+      <c r="C32" t="s">
+        <v>44</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F32" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" ht="68" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>52</v>
+      </c>
+      <c r="D33" t="s">
+        <v>53</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F33" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C41" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adding book1 consisting of leetcode solving tricks according to patterns
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/namankothari/Documents/Naman Kothari/Leetcode_Solutions/Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60A3F46E-EA21-EB43-8B05-6CFA49A11551}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0628800C-FA24-794D-8AA7-D6607F3D61F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3480" yWindow="2560" windowWidth="27640" windowHeight="16940" xr2:uid="{C34AE6C3-BFC3-4D45-AF40-CB304CD30E76}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="68">
   <si>
     <t>Binary Search Tree</t>
   </si>
@@ -269,6 +269,15 @@
   </si>
   <si>
     <t>if it was rather from a left to right range instead of n-1 then it is a famous leetcode question called "its called "Range Sum Query - Immutable" on leetcode"</t>
+  </si>
+  <si>
+    <t>Union Find</t>
+  </si>
+  <si>
+    <t>It is an algorithm specifically made for "DISJOINT" / "CONNECTED" components count/identification, so the moment you see such keywords, consider UNION FIND TOO!!</t>
+  </si>
+  <si>
+    <t>whenever you do union find you are finding the ROOT PARENT and not just any parent, remember this</t>
   </si>
 </sst>
 </file>
@@ -912,10 +921,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B3C76B8-389E-4747-9BF7-DE3D6AB721EC}">
-  <dimension ref="A1:K41"/>
+  <dimension ref="A1:K68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="D68" sqref="D68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1182,6 +1191,17 @@
         <v>46</v>
       </c>
     </row>
+    <row r="68" spans="2:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="B68" t="s">
+        <v>65</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D68" t="s">
+        <v>67</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
adding LPS trick to the dp section
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/namankothari/Documents/Naman Kothari/Leetcode_Solutions/Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{466B0E4C-FBCB-1D4A-92B8-98996C8BF17C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9510503-0394-C341-9A16-7AFBCEE5998F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="21360" xr2:uid="{C34AE6C3-BFC3-4D45-AF40-CB304CD30E76}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="74">
   <si>
     <t>Binary Search Tree</t>
   </si>
@@ -325,6 +325,12 @@
 # 4- draw out the dependencies and make sure that you have got all the dependencies you need to proceed further
 # 5- Check for constraints.</t>
     </r>
+  </si>
+  <si>
+    <t>1- Longest palindromic substring</t>
+  </si>
+  <si>
+    <t>go through each of the letter in the word and span outwards in both the directions to check if it’s a palindrome or not and if it is then get the index f the longest length and so can use this to reduce the TC.</t>
   </si>
 </sst>
 </file>
@@ -976,10 +982,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B3C76B8-389E-4747-9BF7-DE3D6AB721EC}">
-  <dimension ref="A1:K70"/>
+  <dimension ref="A1:K72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="D70" sqref="D70"/>
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="B73" sqref="B73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1271,6 +1277,14 @@
         <v>69</v>
       </c>
     </row>
+    <row r="72" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="B72" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
added longest increasing subsequence solution
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/namankothari/Documents/Naman Kothari/Leetcode_Solutions/Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{462C9EB4-091D-2242-9234-241032D20109}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C44C7901-CFAF-7143-A4AD-536EAB2B5EFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="21360" xr2:uid="{C34AE6C3-BFC3-4D45-AF40-CB304CD30E76}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="82">
   <si>
     <t>Binary Search Tree</t>
   </si>
@@ -398,6 +398,14 @@
   </si>
   <si>
     <t>can this be done(true/false) when comparing substrings to segmented words</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4- longest increasing subsequence </t>
+  </si>
+  <si>
+    <t>For O(n log n) Binary Search Solution:
+Trick Learned:
+Instead of keeping an actual subsequence, keep track of the smallest possible tail values of increasing subsequences of different lengths. If a new number can replace an existing element (using binary search) while maintaining order, do so! This helps ensure that your sequence stays optimized while still tracking valid LIS lengths.</t>
   </si>
 </sst>
 </file>
@@ -1055,10 +1063,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B3C76B8-389E-4747-9BF7-DE3D6AB721EC}">
-  <dimension ref="A1:K75"/>
+  <dimension ref="A1:K76"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="B76" sqref="B76"/>
+      <selection activeCell="D76" sqref="D76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1380,6 +1388,14 @@
         <v>79</v>
       </c>
     </row>
+    <row r="76" spans="1:5" ht="102" x14ac:dyDescent="0.2">
+      <c r="B76" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>